<commit_message>
cas de test pret/ securite pages / Docum securite pages / docum hierarchie onglet
</commit_message>
<xml_diff>
--- a/Requis_Remise/Cas de test/Testes_partie mick.xlsx
+++ b/Requis_Remise/Cas de test/Testes_partie mick.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Liste inventaires (205)" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17207" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17267" uniqueCount="464">
   <si>
     <t>Cas de test</t>
   </si>
@@ -1369,6 +1369,87 @@
   <si>
     <t>S-Médicament-3</t>
   </si>
+  <si>
+    <t>Tests sur les prêts d'équipements</t>
+  </si>
+  <si>
+    <t>T-Pret-1</t>
+  </si>
+  <si>
+    <t>T-Pret-2</t>
+  </si>
+  <si>
+    <t>T-Pret-3</t>
+  </si>
+  <si>
+    <t>T-Pret-4</t>
+  </si>
+  <si>
+    <t>S-Pret-1</t>
+  </si>
+  <si>
+    <t>S-Pret-2</t>
+  </si>
+  <si>
+    <t>La Section prêt d'équipment n'est pas visible</t>
+  </si>
+  <si>
+    <t>La Section prêt d'équipment est visible</t>
+  </si>
+  <si>
+    <t>Camisole --&gt; Rien saisir</t>
+  </si>
+  <si>
+    <t>(290) Cliquer sur l'icône de Donald Ron</t>
+  </si>
+  <si>
+    <t>Saisir 5-6 H Bleu Large 14 comme camisole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saisir Small comme short </t>
+  </si>
+  <si>
+    <t>Saisir 24-02-2017 comme date de prêt</t>
+  </si>
+  <si>
+    <t>Saisir 17-03-2017 comme Date prévue du retour</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton Ajouter Prêt</t>
+  </si>
+  <si>
+    <t>S-Pret-3</t>
+  </si>
+  <si>
+    <t>Choisir la camisole saisie au scénario S-Pret-2</t>
+  </si>
+  <si>
+    <t>Choisir le short saisie au scénario S-Pret-2</t>
+  </si>
+  <si>
+    <t>La camisole est absente dans la liste</t>
+  </si>
+  <si>
+    <t>Le short est absent dans la liste</t>
+  </si>
+  <si>
+    <t>Saisir le prêt créé au scénario S-Pret-2</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton Recevoir Prêt</t>
+  </si>
+  <si>
+    <t>S-Pret-4</t>
+  </si>
+  <si>
+    <t>S-Pret-5</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton Supprimer Prêt</t>
+  </si>
+  <si>
+    <t>La date de réception devient la date d'aujourd'hui</t>
+  </si>
 </sst>
 </file>
 
@@ -1838,24 +1919,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1865,15 +1928,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1914,6 +1968,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1923,12 +2002,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="155">
+  <dxfs count="170">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2050,974 +2131,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -3271,6 +2384,1216 @@
           <color indexed="64"/>
         </left>
         <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -4220,111 +4543,137 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A4:D14" totalsRowShown="0" headerRowDxfId="154" dataDxfId="152" headerRowBorderDxfId="153" tableBorderDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A4:D14" totalsRowShown="0" headerRowDxfId="169" dataDxfId="167" headerRowBorderDxfId="168" tableBorderDxfId="166">
   <autoFilter ref="A4:D14"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro" dataDxfId="150"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="149"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="148"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="147"/>
+    <tableColumn id="1" name="Numéro" dataDxfId="165"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="164"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="163"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="162"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau13" displayName="Tableau13" ref="A15:D38" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="65" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau13" displayName="Tableau13" ref="A15:D38" totalsRowShown="0" headerRowDxfId="100" headerRowBorderDxfId="99" tableBorderDxfId="98">
   <autoFilter ref="A15:D38"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="64"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="63"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="62"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="61"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="97"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="96"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="95"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau3122315" displayName="Tableau3122315" ref="A4:D6" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau3122315" displayName="Tableau3122315" ref="A4:D6" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
   <autoFilter ref="A4:D6"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="18"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="17"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="16"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="15"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="89"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="88"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="87"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau1317" displayName="Tableau1317" ref="A10:D28" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="57" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau1317" displayName="Tableau1317" ref="A10:D28" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83">
   <autoFilter ref="A10:D28"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="56"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="55"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="54"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="53"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="82"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="81"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="80"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau312231518" displayName="Tableau312231518" ref="A4:D9" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="50" tableBorderDxfId="51" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau312231518" displayName="Tableau312231518" ref="A4:D9" totalsRowShown="0" headerRowDxfId="78" headerRowBorderDxfId="77" tableBorderDxfId="76" totalsRowBorderDxfId="75">
   <autoFilter ref="A4:D9"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="48"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="47"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="46"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="45"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="74"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="73"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="72"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau131719" displayName="Tableau131719" ref="A12:D27" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="42" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau131719" displayName="Tableau131719" ref="A12:D27" totalsRowShown="0" headerRowDxfId="70" headerRowBorderDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="A12:D27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="41"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="40"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="39"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="38"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="67"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="66"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="65"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau31223151820" displayName="Tableau31223151820" ref="A4:D9" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau31223151820" displayName="Tableau31223151820" ref="A4:D9" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <autoFilter ref="A4:D9"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="33"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="32"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="31"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="30"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="59"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="58"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="57"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau13171921" displayName="Tableau13171921" ref="A12:D27" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="27" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau13171921" displayName="Tableau13171921" ref="A12:D27" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="A12:D27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="26"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="25"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="24"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="23"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="52"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="51"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="50"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau3122315182022" displayName="Tableau3122315182022" ref="A4:D8" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau3122315182022" displayName="Tableau3122315182022" ref="A4:D8" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+  <autoFilter ref="A4:D8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Numéro " dataDxfId="44"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="43"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="42"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="41"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau1317192123" displayName="Tableau1317192123" ref="A11:D27" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38">
+  <autoFilter ref="A11:D27"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Numéro " dataDxfId="37"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="36"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="35"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau31223151820228" displayName="Tableau31223151820228" ref="A4:D8" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
   <autoFilter ref="A4:D8"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Numéro " dataDxfId="10"/>
@@ -4336,9 +4685,22 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau1317192123" displayName="Tableau1317192123" ref="A11:D27" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
-  <autoFilter ref="A11:D27"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A23:D44" totalsRowShown="0" headerRowDxfId="161" headerRowBorderDxfId="160" tableBorderDxfId="159">
+  <autoFilter ref="A23:D44"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Numéro " dataDxfId="158"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="157"/>
+    <tableColumn id="3" name="Résultat attendu"/>
+    <tableColumn id="4" name="Résultat obtenu"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tableau131719212324" displayName="Tableau131719212324" ref="A11:D30" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="A11:D30"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Numéro " dataDxfId="3"/>
     <tableColumn id="2" name="Manipulations" dataDxfId="2"/>
@@ -4349,142 +4711,129 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A4:D9" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A4:D9" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A4:D9"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro" dataDxfId="89"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="88"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="87"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="86"/>
+    <tableColumn id="1" name="Numéro" dataDxfId="29"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="28"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="27"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A23:D44" totalsRowShown="0" headerRowDxfId="146" headerRowBorderDxfId="145" tableBorderDxfId="144">
-  <autoFilter ref="A23:D44"/>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A12:D33" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A12:D33"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="143"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="142"/>
-    <tableColumn id="3" name="Résultat attendu"/>
-    <tableColumn id="4" name="Résultat obtenu"/>
+    <tableColumn id="1" name="Numéro" dataDxfId="21"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="20"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="19"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A12:D33" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83" totalsRowBorderDxfId="82">
-  <autoFilter ref="A12:D33"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Numéro" dataDxfId="81"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="80"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="79"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="78"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau15" displayName="Tableau15" ref="A2:B46" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau15" displayName="Tableau15" ref="A2:B46" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:B46"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Numero message"/>
-    <tableColumn id="2" name="Message envoyé" dataDxfId="75"/>
+    <tableColumn id="2" name="Message envoyé" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A4:D20" totalsRowShown="0" headerRowDxfId="141" headerRowBorderDxfId="140" tableBorderDxfId="139" totalsRowBorderDxfId="138">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A4:D20" totalsRowShown="0" headerRowDxfId="156" headerRowBorderDxfId="155" tableBorderDxfId="154" totalsRowBorderDxfId="153">
   <autoFilter ref="A4:D20"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="137"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="136"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="135"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="134"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="152"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="151"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="150"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="149"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A4:D10" totalsRowShown="0" headerRowDxfId="133" headerRowBorderDxfId="132" tableBorderDxfId="131" totalsRowBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A4:D10" totalsRowShown="0" headerRowDxfId="148" headerRowBorderDxfId="147" tableBorderDxfId="146" totalsRowBorderDxfId="145">
   <autoFilter ref="A4:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="129"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="128"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="127"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="126"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="144"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="143"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="142"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="141"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A13:D27" totalsRowShown="0" headerRowDxfId="125" headerRowBorderDxfId="124" tableBorderDxfId="123" totalsRowBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A13:D27" totalsRowShown="0" headerRowDxfId="140" headerRowBorderDxfId="139" tableBorderDxfId="138" totalsRowBorderDxfId="137">
   <autoFilter ref="A13:D27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="121"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="120"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="119"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="118"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="136"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="135"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="134"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="133"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau312" displayName="Tableau312" ref="A4:D12" totalsRowShown="0" headerRowDxfId="117" headerRowBorderDxfId="116" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau312" displayName="Tableau312" ref="A4:D12" totalsRowShown="0" headerRowDxfId="132" headerRowBorderDxfId="131" tableBorderDxfId="130" totalsRowBorderDxfId="129">
   <autoFilter ref="A4:D12"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="113"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="112"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="111"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="110"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="128"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="127"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="126"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau413" displayName="Tableau413" ref="A15:D38" totalsRowShown="0" headerRowDxfId="109" headerRowBorderDxfId="108" tableBorderDxfId="107" totalsRowBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau413" displayName="Tableau413" ref="A15:D38" totalsRowShown="0" headerRowDxfId="124" headerRowBorderDxfId="123" tableBorderDxfId="122" totalsRowBorderDxfId="121">
   <autoFilter ref="A15:D38"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="105"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="104"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="103"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="102"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="120"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="119"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="118"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau3122" displayName="Tableau3122" ref="A4:D13" totalsRowShown="0" headerRowDxfId="101" headerRowBorderDxfId="100" tableBorderDxfId="99" totalsRowBorderDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau3122" displayName="Tableau3122" ref="A4:D13" totalsRowShown="0" headerRowDxfId="116" headerRowBorderDxfId="115" tableBorderDxfId="114" totalsRowBorderDxfId="113">
   <autoFilter ref="A4:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="97"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="96"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="95"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="94"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="112"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="111"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="110"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau31223" displayName="Tableau31223" ref="A4:D12" totalsRowShown="0" headerRowDxfId="74" headerRowBorderDxfId="72" tableBorderDxfId="73" totalsRowBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau31223" displayName="Tableau31223" ref="A4:D12" totalsRowShown="0" headerRowDxfId="108" headerRowBorderDxfId="107" tableBorderDxfId="106" totalsRowBorderDxfId="105">
   <autoFilter ref="A4:D12"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="70"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="69"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="68"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="67"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="104"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="103"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="102"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4769,28 +5118,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>245</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -4966,8 +5315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4979,28 +5328,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>413</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -5034,7 +5383,7 @@
       <c r="B6" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="38" t="s">
         <v>421</v>
       </c>
     </row>
@@ -5068,30 +5417,30 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="67"/>
+      <c r="E11" s="58"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="42" t="s">
         <v>428</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -5105,12 +5454,12 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="1" t="s">
         <v>343</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="54"/>
+      <c r="D13" s="45"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -5119,7 +5468,7 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="42" t="s">
         <v>429</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -5175,7 +5524,7 @@
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="42" t="s">
         <v>436</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -5203,7 +5552,7 @@
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="42" t="s">
         <v>435</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -5213,30 +5562,30 @@
       <c r="D24" s="20"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="1" t="s">
         <v>430</v>
       </c>
       <c r="C25" s="30"/>
-      <c r="D25" s="70"/>
+      <c r="D25" s="61"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="1" t="s">
         <v>431</v>
       </c>
       <c r="C26" s="30"/>
-      <c r="D26" s="70"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
-      <c r="B27" s="32" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="14" t="s">
         <v>433</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="14" t="s">
         <v>433</v>
       </c>
     </row>
@@ -5257,13 +5606,326 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="3" max="4" width="75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>437</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="58"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>442</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="44"/>
+      <c r="B13" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="45"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>443</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
+        <v>453</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
+        <v>460</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="60"/>
+      <c r="B27" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>463</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="60"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="61"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="42" t="s">
+        <v>461</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -5284,28 +5946,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -5392,12 +6054,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -5645,10 +6307,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5881,7 +6543,7 @@
       <c r="A33" t="s">
         <v>321</v>
       </c>
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="55" t="s">
         <v>329</v>
       </c>
     </row>
@@ -5889,7 +6551,7 @@
       <c r="A34" t="s">
         <v>331</v>
       </c>
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="56" t="s">
         <v>330</v>
       </c>
     </row>
@@ -5919,7 +6581,7 @@
       <c r="A39" t="s">
         <v>365</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="34" t="s">
         <v>368</v>
       </c>
     </row>
@@ -5927,7 +6589,7 @@
       <c r="A40" t="s">
         <v>366</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="35" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5935,18 +6597,18 @@
       <c r="B41" s="15"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="36" t="s">
         <v>388</v>
       </c>
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="54" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="36" t="s">
         <v>389</v>
       </c>
-      <c r="B43" s="62" t="s">
+      <c r="B43" s="53" t="s">
         <v>391</v>
       </c>
     </row>
@@ -5957,15 +6619,15 @@
       <c r="A45" t="s">
         <v>420</v>
       </c>
-      <c r="B45" s="63" t="s">
+      <c r="B45" s="54" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="38" t="s">
         <v>421</v>
       </c>
-      <c r="B46" s="75" t="s">
+      <c r="B46" s="63" t="s">
         <v>423</v>
       </c>
     </row>
@@ -5999,28 +6661,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -6270,12 +6932,12 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -6528,28 +7190,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -6656,12 +7318,12 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -6859,28 +7521,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -7015,12 +7677,12 @@
       <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -7302,28 +7964,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -7495,28 +8157,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -7646,30 +8308,30 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="71"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="41" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="42" t="s">
         <v>299</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -7678,78 +8340,78 @@
       <c r="C16" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="D16" s="52" t="s">
+      <c r="D16" s="43" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="1" t="s">
         <v>301</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="45"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="1" t="s">
         <v>302</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="54"/>
+      <c r="D19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="1" t="s">
         <v>306</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="54"/>
+      <c r="D20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="1" t="s">
         <v>305</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="54"/>
+      <c r="D21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="1" t="s">
         <v>303</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="54"/>
+      <c r="D22" s="45"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="1" t="s">
         <v>185</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="45" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="54"/>
+      <c r="D24" s="45"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="44" t="s">
         <v>309</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -7758,46 +8420,46 @@
       <c r="C25" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="45" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="1" t="s">
         <v>311</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="54"/>
+      <c r="D26" s="45"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="1" t="s">
         <v>312</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="54"/>
+      <c r="D27" s="45"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="37" t="s">
         <v>315</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="46" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="54"/>
+      <c r="D29" s="45"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="44" t="s">
         <v>313</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -7806,38 +8468,38 @@
       <c r="C30" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D30" s="54" t="s">
+      <c r="D30" s="45" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="1" t="s">
         <v>314</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="54"/>
+      <c r="D31" s="45"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D32" s="45" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="54"/>
+      <c r="D33" s="45"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="44" t="s">
         <v>317</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -7846,55 +8508,55 @@
       <c r="C34" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D34" s="54" t="s">
+      <c r="D34" s="45" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="30" t="s">
         <v>143</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="56" t="s">
+      <c r="D35" s="47" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="14" t="s">
         <v>147</v>
       </c>
       <c r="C36" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="48" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="30" t="s">
         <v>143</v>
       </c>
       <c r="C37" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="56" t="s">
+      <c r="D37" s="47" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="58"/>
-      <c r="B38" s="59" t="s">
+      <c r="A38" s="49"/>
+      <c r="B38" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="C38" s="60" t="s">
+      <c r="C38" s="51" t="s">
         <v>319</v>
       </c>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="52" t="s">
         <v>320</v>
       </c>
       <c r="E38" s="29" t="s">
@@ -7933,28 +8595,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -57156,22 +57818,22 @@
       <c r="D9" s="74"/>
     </row>
     <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="67"/>
+      <c r="E10" s="58"/>
     </row>
     <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="42" t="s">
         <v>342</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -57180,19 +57842,19 @@
       <c r="C11" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="43" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:16384" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="1" t="s">
         <v>343</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="45" t="s">
         <v>307</v>
       </c>
     </row>
@@ -57376,28 +58038,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>386</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -57479,30 +58141,30 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="67"/>
+      <c r="E12" s="58"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="42" t="s">
         <v>374</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -57516,12 +58178,12 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="1" t="s">
         <v>343</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="54"/>
+      <c r="D14" s="45"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -57530,7 +58192,7 @@
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="42" t="s">
         <v>375</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -57586,7 +58248,7 @@
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="59" t="s">
         <v>381</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -57614,7 +58276,7 @@
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="59" t="s">
         <v>384</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -57624,15 +58286,15 @@
       <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="30" t="s">
         <v>377</v>
       </c>
       <c r="C26" s="30"/>
-      <c r="D26" s="70"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="32" t="s">
         <v>380</v>
       </c>
@@ -57675,28 +58337,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="65" t="s">
         <v>387</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -57719,7 +58381,7 @@
       <c r="B5" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="36" t="s">
         <v>388</v>
       </c>
     </row>
@@ -57730,7 +58392,7 @@
       <c r="B6" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="36" t="s">
         <v>389</v>
       </c>
     </row>
@@ -57778,30 +58440,30 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="67"/>
+      <c r="E12" s="58"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="42" t="s">
         <v>405</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -57815,12 +58477,12 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="1" t="s">
         <v>343</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="54"/>
+      <c r="D14" s="45"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -57829,7 +58491,7 @@
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="42" t="s">
         <v>407</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -57885,7 +58547,7 @@
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="42" t="s">
         <v>406</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -57913,7 +58575,7 @@
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="59" t="s">
         <v>408</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -57923,15 +58585,15 @@
       <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="1" t="s">
         <v>410</v>
       </c>
       <c r="C26" s="30"/>
-      <c r="D26" s="70"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="32" t="s">
         <v>411</v>
       </c>

</xml_diff>